<commit_message>
Insertion des descriptions des messages
par les stagiaires : EL-KASMI HAMZA et OUSSAMA KARABILA
</commit_message>
<xml_diff>
--- a/TDM103 - Affectation des messages.xlsx
+++ b/TDM103 - Affectation des messages.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESSARRAJ.FOUAD\Google Drive\Formations\Modules\Programmation Structuré\Rapport_Exceptions\TDM 103\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FDCD7D4-FD36-492E-AA18-680E0614CD36}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{7655B60F-5F9C-47B6-B870-03746E734E53}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TDM 103 - Messages" sheetId="1" r:id="rId1"/>
+    <sheet name="Messages" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TDM 103 - Messages'!$A$1:$C$30</definedName>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>Nom</t>
   </si>
@@ -244,13 +239,34 @@
   </si>
   <si>
     <t>M15</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>autres</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>C#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +308,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -319,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -364,11 +388,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -386,6 +438,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,7 +483,7 @@
         <xdr:cNvPr id="2" name="AutoShape 1" descr="https://cplus.ismontic.ma/Upload/319336d8-ebd5-4340-88c3-19b68b3091fd/Small.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{268F25E5-8EB2-480A-9CA2-0A663EF99F17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{268F25E5-8EB2-480A-9CA2-0A663EF99F17}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -462,7 +526,7 @@
         <xdr:cNvPr id="3" name="AutoShape 3" descr="https://cplus.ismontic.ma/Upload/99b0fa68-39b5-4549-8946-6d735abe00be/Small.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24E7DCC5-05C7-4A12-B8EE-F34F5F79DCFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24E7DCC5-05C7-4A12-B8EE-F34F5F79DCFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -784,20 +848,20 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3388BBFC-84DF-4743-B98F-265CE9C79CFE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="78.75" customHeight="1" x14ac:dyDescent="1.35"/>
@@ -1095,7 +1159,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C30" xr:uid="{3ECC0AC2-7EF3-4758-AF1A-7A16B814E60E}">
+  <autoFilter ref="A1:C30">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1106,4 +1170,342 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8">
+        <v>7.1</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8">
+        <v>8</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8">
+        <v>5</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8">
+        <v>9</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="11">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8">
+        <v>13</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8">
+        <v>14</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>-1</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>-2</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>